<commit_message>
Fix to Library conversion container kind drop down.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_conversion_v4_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_conversion_v4_4_0.xlsx
@@ -848,7 +848,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="24.78"/>
@@ -8746,7 +8746,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.67"/>
@@ -21918,7 +21918,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5:H480" type="list">
       <formula1>Index!$E$2:$E$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -21946,13 +21946,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.99"/>
   </cols>
@@ -22312,7 +22312,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.78"/>

</xml_diff>